<commit_message>
Update PT Emergency Medicine v2.xlsx
</commit_message>
<xml_diff>
--- a/data/PT Emergency Medicine v2.xlsx
+++ b/data/PT Emergency Medicine v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petey\Desktop\sim\sim with jim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\court\OneDrive\Documents\GitHub\em-quiz-game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C736EB10-037B-4CCB-8F61-8A10DDC98A30}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1147">
   <si>
     <t>values per American Board of Emergency Medicine</t>
   </si>
@@ -3613,6 +3613,18 @@
   </si>
   <si>
     <t>Negative</t>
+  </si>
+  <si>
+    <t>CBC_WBC</t>
+  </si>
+  <si>
+    <t>CBC_HCT</t>
+  </si>
+  <si>
+    <t>CBC_HGB</t>
+  </si>
+  <si>
+    <t>CBC_Platelets</t>
   </si>
 </sst>
 </file>
@@ -4104,14 +4116,14 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.265625" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4134,7 +4146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -4172,7 +4184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -4201,7 +4213,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -4236,7 +4248,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -4256,7 +4268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
@@ -4294,7 +4306,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>173</v>
       </c>
@@ -4335,12 +4347,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>187</v>
       </c>
@@ -4363,40 +4375,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>258</v>
       </c>
@@ -4404,7 +4416,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>262</v>
       </c>
@@ -4488,7 +4500,7 @@
       </c>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>315</v>
       </c>
@@ -4556,7 +4568,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="60" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="L60" s="1" t="s">
         <v>160</v>
       </c>
@@ -4577,14 +4589,14 @@
       <selection activeCell="A25" sqref="A25:BJ41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.265625" customWidth="1"/>
+    <col min="3" max="3" width="18.86328125" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B1" s="16" t="s">
         <v>744</v>
       </c>
@@ -4598,7 +4610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4672,7 +4684,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
@@ -4780,7 +4792,7 @@
       </c>
       <c r="BF3" s="6"/>
     </row>
-    <row r="4" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -4944,7 +4956,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -5039,7 +5051,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>97</v>
       </c>
@@ -5116,7 +5128,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>106</v>
       </c>
@@ -5193,7 +5205,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>115</v>
       </c>
@@ -5261,7 +5273,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>123</v>
       </c>
@@ -5320,7 +5332,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
         <v>129</v>
       </c>
@@ -5364,7 +5376,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:62" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D11" s="2" t="s">
         <v>137</v>
       </c>
@@ -5402,7 +5414,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:62" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:62" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
         <v>140</v>
       </c>
@@ -5437,7 +5449,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
         <v>147</v>
       </c>
@@ -5466,7 +5478,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D14" s="1" t="s">
         <v>151</v>
       </c>
@@ -5501,7 +5513,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D15" s="1" t="s">
         <v>156</v>
       </c>
@@ -5539,7 +5551,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:62" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D16" s="1" t="s">
         <v>161</v>
       </c>
@@ -5571,7 +5583,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="17" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AY17" s="1" t="s">
         <v>289</v>
       </c>
@@ -5582,7 +5594,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="18" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AY18" s="1" t="s">
         <v>297</v>
       </c>
@@ -5593,7 +5605,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AY19" s="1" t="s">
         <v>302</v>
       </c>
@@ -5604,29 +5616,29 @@
         <v>294</v>
       </c>
     </row>
-    <row r="21" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B24" s="16"/>
       <c r="D24" s="6"/>
       <c r="G24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="51:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="51:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="51:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="51:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="51:53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="51:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="51:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="51:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="51:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="51:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="51:53" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="51:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AY42" s="6" t="s">
         <v>302</v>
       </c>
@@ -5651,22 +5663,22 @@
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="14" max="14" width="20.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" customWidth="1"/>
-    <col min="16" max="16" width="24.5703125" customWidth="1"/>
-    <col min="27" max="27" width="19.5703125" customWidth="1"/>
-    <col min="28" max="28" width="19.28515625" customWidth="1"/>
-    <col min="29" max="29" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="20.3984375" customWidth="1"/>
+    <col min="15" max="15" width="22.59765625" customWidth="1"/>
+    <col min="16" max="16" width="24.59765625" customWidth="1"/>
+    <col min="27" max="27" width="19.59765625" customWidth="1"/>
+    <col min="28" max="28" width="19.265625" customWidth="1"/>
+    <col min="29" max="29" width="18.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:36" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B1" s="14" t="s">
         <v>1097</v>
       </c>
     </row>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B2" s="28" t="s">
         <v>889</v>
       </c>
@@ -5674,7 +5686,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:36" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>794</v>
       </c>
@@ -5694,7 +5706,7 @@
       <c r="R3" s="14"/>
       <c r="V3" s="14"/>
     </row>
-    <row r="4" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>890</v>
       </c>
@@ -5717,7 +5729,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>797</v>
       </c>
@@ -5749,7 +5761,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>891</v>
       </c>
@@ -5781,7 +5793,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
         <v>892</v>
       </c>
@@ -5815,7 +5827,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>803</v>
       </c>
@@ -5850,7 +5862,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="9" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>806</v>
       </c>
@@ -5884,7 +5896,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>875</v>
       </c>
@@ -5912,7 +5924,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
         <v>818</v>
       </c>
@@ -5940,7 +5952,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>893</v>
       </c>
@@ -5971,7 +5983,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="13" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
         <v>874</v>
       </c>
@@ -6001,7 +6013,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.35">
       <c r="D14" s="11"/>
       <c r="F14" s="11" t="s">
         <v>1104</v>
@@ -6019,7 +6031,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:36" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B15" s="28" t="s">
         <v>894</v>
       </c>
@@ -6048,7 +6060,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
         <v>794</v>
       </c>
@@ -6080,7 +6092,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
         <v>895</v>
       </c>
@@ -6112,7 +6124,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
         <v>896</v>
       </c>
@@ -6144,7 +6156,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
         <v>897</v>
       </c>
@@ -6170,7 +6182,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B20" s="28" t="s">
         <v>877</v>
       </c>
@@ -6193,7 +6205,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="s">
         <v>878</v>
       </c>
@@ -6213,7 +6225,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:32" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B22" s="29" t="s">
         <v>880</v>
       </c>
@@ -6230,7 +6242,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:32" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B23" s="18" t="s">
         <v>881</v>
       </c>
@@ -6256,7 +6268,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
         <v>882</v>
       </c>
@@ -6282,7 +6294,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
         <v>794</v>
       </c>
@@ -6302,7 +6314,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
         <v>788</v>
       </c>
@@ -6325,7 +6337,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>883</v>
       </c>
@@ -6348,7 +6360,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
         <v>817</v>
       </c>
@@ -6365,7 +6377,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.35">
       <c r="F29" s="11" t="s">
         <v>1101</v>
       </c>
@@ -6373,7 +6385,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:32" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B30" s="28" t="s">
         <v>907</v>
       </c>
@@ -6387,7 +6399,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B31" s="11" t="s">
         <v>908</v>
       </c>
@@ -6407,7 +6419,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
         <v>909</v>
       </c>
@@ -6424,7 +6436,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:31" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B33" s="11" t="s">
         <v>803</v>
       </c>
@@ -6447,7 +6459,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:31" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B34" s="11" t="s">
         <v>910</v>
       </c>
@@ -6473,7 +6485,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:31" x14ac:dyDescent="0.35">
       <c r="F35" s="11" t="s">
         <v>795</v>
       </c>
@@ -6493,7 +6505,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B36" s="28" t="s">
         <v>225</v>
       </c>
@@ -6510,7 +6522,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B37" s="11" t="s">
         <v>342</v>
       </c>
@@ -6520,7 +6532,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B38" s="11" t="s">
         <v>850</v>
       </c>
@@ -6528,7 +6540,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B39" s="11" t="s">
         <v>918</v>
       </c>
@@ -6539,7 +6551,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:31" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B40" s="11" t="s">
         <v>919</v>
       </c>
@@ -6556,7 +6568,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B41" s="11" t="s">
         <v>815</v>
       </c>
@@ -6573,7 +6585,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:31" x14ac:dyDescent="0.35">
       <c r="T42" s="11" t="s">
         <v>787</v>
       </c>
@@ -6587,7 +6599,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B43" s="28" t="s">
         <v>929</v>
       </c>
@@ -6604,7 +6616,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:31" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B44" s="14" t="s">
         <v>931</v>
       </c>
@@ -6624,7 +6636,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:31" x14ac:dyDescent="0.35">
       <c r="C45" s="28"/>
       <c r="T45" s="11" t="s">
         <v>786</v>
@@ -6639,7 +6651,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B46" s="28" t="s">
         <v>906</v>
       </c>
@@ -6656,7 +6668,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B47" s="11" t="s">
         <v>850</v>
       </c>
@@ -6670,7 +6682,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B48" s="11" t="s">
         <v>874</v>
       </c>
@@ -6684,7 +6696,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B49" s="11" t="s">
         <v>932</v>
       </c>
@@ -6704,7 +6716,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="50" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="11" t="s">
         <v>340</v>
       </c>
@@ -6724,7 +6736,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B51" s="11" t="s">
         <v>875</v>
       </c>
@@ -6744,7 +6756,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A52" s="27" t="s">
         <v>901</v>
       </c>
@@ -6764,7 +6776,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B53" s="11" t="s">
         <v>800</v>
       </c>
@@ -6785,7 +6797,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A54" s="27" t="s">
         <v>900</v>
       </c>
@@ -6808,7 +6820,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B55" s="11" t="s">
         <v>872</v>
       </c>
@@ -6828,7 +6840,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B56" s="11" t="s">
         <v>902</v>
       </c>
@@ -6851,7 +6863,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A57" s="27" t="s">
         <v>901</v>
       </c>
@@ -6880,7 +6892,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B58" s="11" t="s">
         <v>904</v>
       </c>
@@ -6906,7 +6918,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.35">
       <c r="T59" s="11" t="s">
         <v>796</v>
       </c>
@@ -6926,7 +6938,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B60" s="14" t="s">
         <v>876</v>
       </c>
@@ -6937,12 +6949,12 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B61" s="26" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>850</v>
       </c>
@@ -6950,7 +6962,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>859</v>
       </c>
@@ -6964,7 +6976,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>857</v>
       </c>
@@ -6978,7 +6990,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:40" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>860</v>
       </c>
@@ -6998,7 +7010,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="66" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="26" t="s">
         <v>861</v>
       </c>
@@ -7021,7 +7033,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>862</v>
       </c>
@@ -7044,7 +7056,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="68" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>800</v>
       </c>
@@ -7073,7 +7085,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="69" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>863</v>
       </c>
@@ -7102,7 +7114,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="70" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B70" s="26" t="s">
         <v>864</v>
       </c>
@@ -7125,7 +7137,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>865</v>
       </c>
@@ -7142,7 +7154,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="72" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>866</v>
       </c>
@@ -7156,7 +7168,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="73" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>824</v>
       </c>
@@ -7173,7 +7185,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="74" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>867</v>
       </c>
@@ -7193,7 +7205,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="75" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>868</v>
       </c>
@@ -7213,7 +7225,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B76" s="26" t="s">
         <v>869</v>
       </c>
@@ -7242,7 +7254,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>870</v>
       </c>
@@ -7280,7 +7292,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>871</v>
       </c>
@@ -7315,7 +7327,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>872</v>
       </c>
@@ -7344,7 +7356,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="80" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="26" t="s">
         <v>873</v>
       </c>
@@ -7376,7 +7388,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>874</v>
       </c>
@@ -7405,7 +7417,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B82" s="11" t="s">
         <v>994</v>
       </c>
@@ -7434,7 +7446,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>340</v>
       </c>
@@ -7463,7 +7475,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>875</v>
       </c>
@@ -7492,7 +7504,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>820</v>
       </c>
@@ -7527,7 +7539,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:41" x14ac:dyDescent="0.35">
       <c r="J86" t="s">
         <v>1084</v>
       </c>
@@ -7559,7 +7571,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B87" s="28" t="s">
         <v>885</v>
       </c>
@@ -7582,7 +7594,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="88" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="11" t="s">
         <v>798</v>
       </c>
@@ -7611,7 +7623,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B89" s="11" t="s">
         <v>799</v>
       </c>
@@ -7643,7 +7655,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="90" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B90" s="11" t="s">
         <v>803</v>
       </c>
@@ -7669,7 +7681,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="91" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B91" s="11" t="s">
         <v>818</v>
       </c>
@@ -7695,7 +7707,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="92" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B92" s="11" t="s">
         <v>886</v>
       </c>
@@ -7721,7 +7733,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="93" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B93" s="11" t="s">
         <v>811</v>
       </c>
@@ -7747,7 +7759,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="94" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B94" s="11" t="s">
         <v>812</v>
       </c>
@@ -7773,7 +7785,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="95" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T95" t="s">
         <v>1038</v>
       </c>
@@ -7793,7 +7805,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="96" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B96" s="28" t="s">
         <v>920</v>
       </c>
@@ -7810,7 +7822,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="97" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="11" t="s">
         <v>342</v>
       </c>
@@ -7827,7 +7839,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="98" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B98" s="11" t="s">
         <v>919</v>
       </c>
@@ -7850,7 +7862,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="99" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B99" s="11" t="s">
         <v>815</v>
       </c>
@@ -7870,7 +7882,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="100" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:41" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B100" s="14" t="s">
         <v>792</v>
       </c>
@@ -7884,7 +7896,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="101" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T101" t="s">
         <v>943</v>
       </c>
@@ -7895,7 +7907,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="102" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T102" t="s">
         <v>1041</v>
       </c>
@@ -7909,7 +7921,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="103" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T103" t="s">
         <v>1042</v>
       </c>
@@ -7923,7 +7935,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="104" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T104" t="s">
         <v>1043</v>
       </c>
@@ -7934,7 +7946,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="105" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T105" t="s">
         <v>1037</v>
       </c>
@@ -7945,7 +7957,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="106" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:41" x14ac:dyDescent="0.35">
       <c r="T106" t="s">
         <v>938</v>
       </c>
@@ -7956,7 +7968,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="107" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI107" t="s">
         <v>1083</v>
       </c>
@@ -7964,7 +7976,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="108" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI108" t="s">
         <v>937</v>
       </c>
@@ -7972,7 +7984,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="109" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI109" t="s">
         <v>938</v>
       </c>
@@ -7980,7 +7992,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="110" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI110" t="s">
         <v>941</v>
       </c>
@@ -7988,7 +8000,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="111" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI111" t="s">
         <v>1040</v>
       </c>
@@ -7996,7 +8008,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="112" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:41" x14ac:dyDescent="0.35">
       <c r="AI112" t="s">
         <v>963</v>
       </c>
@@ -8004,7 +8016,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="113" spans="35:36" x14ac:dyDescent="0.2">
+    <row r="113" spans="35:36" x14ac:dyDescent="0.35">
       <c r="AI113" t="s">
         <v>1037</v>
       </c>
@@ -8012,7 +8024,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="114" spans="35:36" x14ac:dyDescent="0.2">
+    <row r="114" spans="35:36" x14ac:dyDescent="0.35">
       <c r="AI114" t="s">
         <v>947</v>
       </c>
@@ -8020,7 +8032,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="115" spans="35:36" x14ac:dyDescent="0.2">
+    <row r="115" spans="35:36" x14ac:dyDescent="0.35">
       <c r="AI115" t="s">
         <v>1095</v>
       </c>
@@ -8028,7 +8040,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="116" spans="35:36" x14ac:dyDescent="0.2">
+    <row r="116" spans="35:36" x14ac:dyDescent="0.35">
       <c r="AI116" t="s">
         <v>950</v>
       </c>
@@ -8036,13 +8048,13 @@
         <v>615</v>
       </c>
     </row>
-    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T166" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="167" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="167" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T167" t="s">
         <v>1073</v>
       </c>
@@ -8050,7 +8062,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="168" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="168" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T168" t="s">
         <v>1074</v>
       </c>
@@ -8058,7 +8070,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="169" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="169" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T169" t="s">
         <v>795</v>
       </c>
@@ -8066,12 +8078,12 @@
         <v>636</v>
       </c>
     </row>
-    <row r="171" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="171" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T171" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="172" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="172" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T172" t="s">
         <v>1075</v>
       </c>
@@ -8079,7 +8091,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="173" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="173" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T173" t="s">
         <v>1076</v>
       </c>
@@ -8087,7 +8099,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="174" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="174" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T174" t="s">
         <v>1077</v>
       </c>
@@ -8095,7 +8107,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="175" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="175" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T175" t="s">
         <v>1078</v>
       </c>
@@ -8103,7 +8115,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="176" spans="20:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="20:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T176" t="s">
         <v>1027</v>
       </c>
@@ -8111,7 +8123,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="177" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="177" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T177" t="s">
         <v>1079</v>
       </c>
@@ -8119,7 +8131,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="178" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="178" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T178" t="s">
         <v>1080</v>
       </c>
@@ -8127,7 +8139,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="179" spans="20:21" x14ac:dyDescent="0.2">
+    <row r="179" spans="20:21" x14ac:dyDescent="0.35">
       <c r="T179" t="s">
         <v>1081</v>
       </c>
@@ -8135,12 +8147,12 @@
         <v>629</v>
       </c>
     </row>
-    <row r="198" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="198" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N198" t="s">
         <v>1082</v>
       </c>
     </row>
-    <row r="199" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="199" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N199" t="s">
         <v>1083</v>
       </c>
@@ -8148,7 +8160,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="200" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="200" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N200" t="s">
         <v>1084</v>
       </c>
@@ -8156,7 +8168,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="201" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="201" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N201" t="s">
         <v>943</v>
       </c>
@@ -8164,7 +8176,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="202" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="202" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N202" t="s">
         <v>950</v>
       </c>
@@ -8172,12 +8184,12 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="204" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="204" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N204" t="s">
         <v>1085</v>
       </c>
     </row>
-    <row r="205" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="205" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N205" t="s">
         <v>1086</v>
       </c>
@@ -8185,7 +8197,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="206" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="206" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N206" t="s">
         <v>1061</v>
       </c>
@@ -8193,17 +8205,17 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="207" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="207" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N207" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="209" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="209" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N209" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="210" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="210" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N210" t="s">
         <v>1035</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="211" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="211" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N211" t="s">
         <v>1088</v>
       </c>
@@ -8219,7 +8231,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="212" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="212" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N212" t="s">
         <v>1089</v>
       </c>
@@ -8227,7 +8239,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="213" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="213" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N213" t="s">
         <v>1090</v>
       </c>
@@ -8235,7 +8247,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="214" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="214" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N214" t="s">
         <v>1091</v>
       </c>
@@ -8243,12 +8255,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="216" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="216" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N216" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="217" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="217" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N217" t="s">
         <v>1092</v>
       </c>
@@ -8256,7 +8268,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="218" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="218" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N218" t="s">
         <v>1093</v>
       </c>
@@ -8264,7 +8276,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="219" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="219" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N219" t="s">
         <v>1094</v>
       </c>
@@ -8272,7 +8284,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="220" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="220" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N220" t="s">
         <v>1043</v>
       </c>
@@ -8280,7 +8292,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="221" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="221" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N221" t="s">
         <v>936</v>
       </c>
@@ -8288,7 +8300,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="222" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="222" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N222" t="s">
         <v>1083</v>
       </c>
@@ -8296,7 +8308,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="223" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="223" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N223" t="s">
         <v>937</v>
       </c>
@@ -8304,7 +8316,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="224" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="224" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N224" t="s">
         <v>938</v>
       </c>
@@ -8312,7 +8324,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="225" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="225" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N225" t="s">
         <v>941</v>
       </c>
@@ -8320,7 +8332,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="226" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="226" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N226" t="s">
         <v>1040</v>
       </c>
@@ -8328,7 +8340,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="227" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="227" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N227" t="s">
         <v>963</v>
       </c>
@@ -8336,7 +8348,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="228" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="228" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N228" t="s">
         <v>1037</v>
       </c>
@@ -8344,7 +8356,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="229" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="229" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N229" t="s">
         <v>947</v>
       </c>
@@ -8352,7 +8364,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="230" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="230" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N230" t="s">
         <v>1095</v>
       </c>
@@ -8360,7 +8372,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="231" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="231" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N231" t="s">
         <v>950</v>
       </c>
@@ -8385,19 +8397,19 @@
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.73046875" customWidth="1"/>
+    <col min="2" max="2" width="26.86328125" customWidth="1"/>
+    <col min="3" max="3" width="41.59765625" customWidth="1"/>
+    <col min="4" max="4" width="36.59765625" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.3984375" customWidth="1"/>
     <col min="7" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>774</v>
       </c>
@@ -8410,7 +8422,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -8422,7 +8434,7 @@
       <c r="I2" s="6"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
         <v>67</v>
       </c>
@@ -8508,7 +8520,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>111</v>
       </c>
@@ -8594,7 +8606,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
         <v>145</v>
       </c>
@@ -8680,7 +8692,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>157</v>
       </c>
@@ -8764,7 +8776,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>179</v>
       </c>
@@ -8848,7 +8860,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>188</v>
       </c>
@@ -8930,7 +8942,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>216</v>
       </c>
@@ -9010,7 +9022,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>768</v>
       </c>
@@ -9082,7 +9094,7 @@
       <c r="AA10" s="11"/>
       <c r="AB10" s="11"/>
     </row>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>243</v>
       </c>
@@ -9152,7 +9164,7 @@
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="31" t="s">
         <v>260</v>
       </c>
@@ -9218,7 +9230,7 @@
       <c r="AA12" s="11"/>
       <c r="AB12" s="11"/>
     </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>185</v>
       </c>
@@ -9282,7 +9294,7 @@
       <c r="AA13" s="11"/>
       <c r="AB13" s="11"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>304</v>
       </c>
@@ -9344,7 +9356,7 @@
       <c r="AA14" s="11"/>
       <c r="AB14" s="11"/>
     </row>
-    <row r="15" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>316</v>
       </c>
@@ -9400,7 +9412,7 @@
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>325</v>
       </c>
@@ -9450,7 +9462,7 @@
       <c r="AA16" s="11"/>
       <c r="AB16" s="11"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>339</v>
       </c>
@@ -9502,7 +9514,7 @@
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="22" t="s">
@@ -9550,7 +9562,7 @@
       <c r="AA18" s="11"/>
       <c r="AB18" s="11"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="22" t="s">
@@ -9598,7 +9610,7 @@
       <c r="AA19" s="11"/>
       <c r="AB19" s="11"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="11"/>
       <c r="C20" s="16" t="s">
@@ -9646,7 +9658,7 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
     </row>
-    <row r="21" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -9690,7 +9702,7 @@
       <c r="AA21" s="11"/>
       <c r="AB21" s="11"/>
     </row>
-    <row r="22" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -9730,7 +9742,7 @@
       <c r="AA22" s="11"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="23" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -9768,7 +9780,7 @@
       <c r="AA23" s="11"/>
       <c r="AB23" s="11"/>
     </row>
-    <row r="24" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -9802,7 +9814,7 @@
       <c r="AA24" s="11"/>
       <c r="AB24" s="11"/>
     </row>
-    <row r="25" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -9836,7 +9848,7 @@
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
     </row>
-    <row r="26" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -9870,7 +9882,7 @@
       <c r="AA26" s="11"/>
       <c r="AB26" s="11"/>
     </row>
-    <row r="27" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -9902,7 +9914,7 @@
       <c r="AA27" s="11"/>
       <c r="AB27" s="11"/>
     </row>
-    <row r="28" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -9934,7 +9946,7 @@
       <c r="AA28" s="11"/>
       <c r="AB28" s="11"/>
     </row>
-    <row r="29" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="16"/>
@@ -9966,7 +9978,7 @@
       <c r="AA29" s="11"/>
       <c r="AB29" s="11"/>
     </row>
-    <row r="30" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -9998,7 +10010,7 @@
       <c r="AA30" s="11"/>
       <c r="AB30" s="11"/>
     </row>
-    <row r="31" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -10028,7 +10040,7 @@
       <c r="AA31" s="11"/>
       <c r="AB31" s="11"/>
     </row>
-    <row r="32" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -10058,64 +10070,64 @@
       <c r="AA32" s="11"/>
       <c r="AB32" s="11"/>
     </row>
-    <row r="33" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I33" s="6"/>
       <c r="S33" s="6"/>
     </row>
-    <row r="34" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C35" s="4"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I37" s="6"/>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I38" s="6"/>
       <c r="T38" s="4"/>
     </row>
-    <row r="39" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I39" s="6"/>
       <c r="R39" s="6"/>
       <c r="T39" s="4"/>
       <c r="U39" s="6"/>
     </row>
-    <row r="40" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I40" s="6"/>
       <c r="R40" s="6"/>
       <c r="T40" s="4"/>
     </row>
-    <row r="41" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I41" s="6"/>
       <c r="S41" s="6"/>
     </row>
-    <row r="42" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I42" s="6"/>
       <c r="S42" s="6"/>
     </row>
-    <row r="43" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="I43" s="6"/>
       <c r="S43" s="6"/>
     </row>
-    <row r="44" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E44" s="4"/>
       <c r="I44" s="6"/>
       <c r="S44" s="6"/>
     </row>
-    <row r="45" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="S45" s="6"/>
     </row>
-    <row r="46" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -10123,14 +10135,14 @@
       <c r="S46" s="6"/>
       <c r="U46" s="6"/>
     </row>
-    <row r="47" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="S47" s="6"/>
       <c r="U47" s="6"/>
     </row>
-    <row r="48" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="6"/>
@@ -10138,7 +10150,7 @@
       <c r="S48" s="6"/>
       <c r="U48" s="6"/>
     </row>
-    <row r="49" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="6"/>
@@ -10146,56 +10158,56 @@
       <c r="S49" s="6"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G50" s="4"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="S50" s="6"/>
       <c r="U50" s="6"/>
     </row>
-    <row r="51" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G51" s="4"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="S51" s="6"/>
       <c r="U51" s="6"/>
     </row>
-    <row r="52" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G52" s="4"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="S52" s="6"/>
       <c r="U52" s="6"/>
     </row>
-    <row r="53" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G53" s="4"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="S53" s="6"/>
       <c r="U53" s="6"/>
     </row>
-    <row r="54" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G54" s="4"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="S54" s="6"/>
       <c r="U54" s="6"/>
     </row>
-    <row r="55" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G55" s="4"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="S55" s="6"/>
       <c r="U55" s="6"/>
     </row>
-    <row r="56" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="G56" s="4"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="S56" s="6"/>
       <c r="U56" s="6"/>
     </row>
-    <row r="57" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E57" s="6"/>
       <c r="G57" s="4"/>
       <c r="H57" s="6"/>
@@ -10203,7 +10215,7 @@
       <c r="S57" s="6"/>
       <c r="U57" s="6"/>
     </row>
-    <row r="58" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E58" s="6"/>
       <c r="G58" s="4"/>
       <c r="H58" s="6"/>
@@ -10211,7 +10223,7 @@
       <c r="S58" s="6"/>
       <c r="U58" s="6"/>
     </row>
-    <row r="59" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E59" s="6"/>
       <c r="G59" s="4"/>
       <c r="H59" s="6"/>
@@ -10219,7 +10231,7 @@
       <c r="S59" s="6"/>
       <c r="U59" s="6"/>
     </row>
-    <row r="60" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
@@ -10227,7 +10239,7 @@
       <c r="S60" s="6"/>
       <c r="U60" s="6"/>
     </row>
-    <row r="61" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E61" s="6"/>
       <c r="G61" s="4"/>
       <c r="H61" s="6"/>
@@ -10236,63 +10248,63 @@
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
     </row>
-    <row r="62" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="3:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E67" s="4"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="E68" s="4"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="E69" s="4"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="E70" s="4"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="E71" s="4"/>
       <c r="F71" s="6"/>
@@ -10300,7 +10312,7 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="E72" s="4"/>
       <c r="F72" s="6"/>
@@ -10308,7 +10320,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="E73" s="4"/>
       <c r="F73" s="6"/>
@@ -10316,7 +10328,7 @@
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="E74" s="4"/>
       <c r="F74" s="6"/>
@@ -10324,7 +10336,7 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="E75" s="4"/>
       <c r="F75" s="6"/>
@@ -10332,7 +10344,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="E76" s="4"/>
       <c r="F76" s="6"/>
@@ -10340,7 +10352,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="E77" s="4"/>
       <c r="F77" s="6"/>
@@ -10348,7 +10360,7 @@
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
@@ -10356,7 +10368,7 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="E79" s="4"/>
       <c r="F79" s="6"/>
@@ -10364,7 +10376,7 @@
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="E80" s="4"/>
       <c r="F80" s="6"/>
@@ -10372,7 +10384,7 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="E81" s="4"/>
       <c r="F81" s="6"/>
@@ -10380,7 +10392,7 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
@@ -10388,7 +10400,7 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -10399,7 +10411,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -10410,7 +10422,7 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -10421,7 +10433,7 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -10432,7 +10444,7 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -10443,7 +10455,7 @@
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -10467,13 +10479,13 @@
   </sheetPr>
   <dimension ref="A1:BX7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AU19" sqref="AU19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>535</v>
       </c>
@@ -10640,7 +10652,7 @@
       <c r="BW1" s="1"/>
       <c r="BX1" s="1"/>
     </row>
-    <row r="2" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10801,7 +10813,7 @@
       <c r="BW2" s="1"/>
       <c r="BX2" s="1"/>
     </row>
-    <row r="3" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10950,7 +10962,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="7" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AK7" s="1" t="s">
         <v>160</v>
       </c>
@@ -10966,15 +10978,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54834C7C-FFC1-4FDA-AF9B-33C488204F5D}">
-  <dimension ref="A1:BJ17"/>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:62" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" ht="39.4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -11048,7 +11060,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>52</v>
       </c>
@@ -11156,7 +11168,7 @@
       </c>
       <c r="BF2" s="6"/>
     </row>
-    <row r="3" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" ht="25.9" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>66</v>
       </c>
@@ -11320,7 +11332,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>86</v>
       </c>
@@ -11415,7 +11427,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>97</v>
       </c>
@@ -11492,7 +11504,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>106</v>
       </c>
@@ -11569,7 +11581,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="D7" s="6" t="s">
         <v>115</v>
@@ -11638,7 +11650,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
       <c r="D8" s="6" t="s">
         <v>123</v>
       </c>
@@ -11697,7 +11709,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="D9" s="6" t="s">
         <v>129</v>
       </c>
@@ -11741,7 +11753,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:62" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D10" s="2" t="s">
         <v>137</v>
       </c>
@@ -11779,7 +11791,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:62" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D11" s="6" t="s">
         <v>140</v>
       </c>
@@ -11814,7 +11826,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
       <c r="D12" s="6" t="s">
         <v>147</v>
       </c>
@@ -11843,7 +11855,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="13" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="D13" s="6" t="s">
         <v>151</v>
       </c>
@@ -11878,7 +11890,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="14" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="D14" s="6" t="s">
         <v>156</v>
       </c>
@@ -11916,7 +11928,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.35">
       <c r="D15" s="6" t="s">
         <v>161</v>
       </c>
@@ -11948,7 +11960,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:62" ht="25.5" x14ac:dyDescent="0.35">
       <c r="AY16" s="6" t="s">
         <v>289</v>
       </c>
@@ -11959,7 +11971,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="51:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.35">
       <c r="AY17" s="6" t="s">
         <v>297</v>
       </c>
@@ -11968,6 +11980,40 @@
       </c>
       <c r="BA17" s="6" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>17000</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -11986,9 +12032,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -12128,7 +12174,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -12296,13 +12342,13 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.59765625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>634</v>
       </c>
@@ -12310,7 +12356,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>639</v>
       </c>
@@ -12321,52 +12367,52 @@
         <v>642</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>655</v>
       </c>
@@ -12387,37 +12433,37 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" customWidth="1"/>
+    <col min="5" max="5" width="54.73046875" customWidth="1"/>
+    <col min="6" max="6" width="4.3984375" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.73046875" customWidth="1"/>
+    <col min="9" max="9" width="29.3984375" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" customWidth="1"/>
+    <col min="11" max="11" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E3" s="1" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E4" s="8" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>672</v>
       </c>
@@ -12440,7 +12486,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>194</v>
       </c>
@@ -12451,7 +12497,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D7" s="1" t="s">
         <v>673</v>
       </c>
@@ -12477,7 +12523,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>673</v>
       </c>
@@ -12491,7 +12537,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>673</v>
       </c>
@@ -12505,7 +12551,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
         <v>673</v>
       </c>
@@ -12516,7 +12562,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>678</v>
       </c>
@@ -12530,7 +12576,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6" t="s">
@@ -12540,7 +12586,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
         <v>673</v>
       </c>
@@ -12554,7 +12600,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F14" s="6" t="s">
         <v>678</v>
       </c>
@@ -12562,7 +12608,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1" t="s">
         <v>673</v>
       </c>
@@ -12570,7 +12616,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D16" s="1" t="s">
         <v>685</v>
       </c>
@@ -12590,7 +12636,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="17" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H17" s="8" t="s">
         <v>678</v>
       </c>
@@ -12599,7 +12645,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H18" s="1" t="s">
         <v>673</v>
       </c>
@@ -12610,32 +12656,32 @@
         <v>691</v>
       </c>
     </row>
-    <row r="19" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K19" s="8" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="20" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K20" s="8" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="21" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K21" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="22" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K22" s="1" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="23" spans="4:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
       <c r="K23" s="1" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="24" spans="4:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D24" s="1" t="s">
         <v>673</v>
       </c>
@@ -12652,7 +12698,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="25" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D25" s="1" t="s">
         <v>673</v>
       </c>

</xml_diff>

<commit_message>
start csv format for labs
</commit_message>
<xml_diff>
--- a/data/PT Emergency Medicine v2.xlsx
+++ b/data/PT Emergency Medicine v2.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\court\OneDrive\Documents\GitHub\em-quiz-game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C736EB10-037B-4CCB-8F61-8A10DDC98A30}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E53566D-913D-4261-9AF7-7C5D5161C518}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="1350" windowWidth="2355" windowHeight="532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1688" yWindow="1688" windowWidth="2355" windowHeight="532" firstSheet="1" activeTab="6" xr2:uid="{E832494E-F55B-4BFD-B915-837CB7A7C282}"/>
   </bookViews>
   <sheets>
     <sheet name="Databases" sheetId="1" r:id="rId1"/>
@@ -19,16 +20,17 @@
     <sheet name="DDx" sheetId="3" r:id="rId4"/>
     <sheet name="Case Info" sheetId="4" r:id="rId5"/>
     <sheet name="Case1 labs" sheetId="9" r:id="rId6"/>
-    <sheet name="CSV Case Info" sheetId="5" r:id="rId7"/>
-    <sheet name="GoalsTasks" sheetId="6" r:id="rId8"/>
-    <sheet name="Flow chart" sheetId="7" r:id="rId9"/>
+    <sheet name="Labs CSV format" sheetId="10" r:id="rId7"/>
+    <sheet name="CSV Case Info" sheetId="5" r:id="rId8"/>
+    <sheet name="GoalsTasks" sheetId="6" r:id="rId9"/>
+    <sheet name="Flow chart" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="1228">
   <si>
     <t>values per American Board of Emergency Medicine</t>
   </si>
@@ -3625,6 +3627,249 @@
   </si>
   <si>
     <t>CBC_Platelets</t>
+  </si>
+  <si>
+    <t>CBCdiff_WBC</t>
+  </si>
+  <si>
+    <t>CBCdiff_HCT</t>
+  </si>
+  <si>
+    <t>CBCdiff_HGB</t>
+  </si>
+  <si>
+    <t>CBCdiff_Platelets</t>
+  </si>
+  <si>
+    <t>CBCdiff_MCV</t>
+  </si>
+  <si>
+    <t>CBCdiff_MCH</t>
+  </si>
+  <si>
+    <t>ColumnName</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>CBCdiff_MCHC</t>
+  </si>
+  <si>
+    <t>CBCdiff_Neutrophils</t>
+  </si>
+  <si>
+    <t>CBCdiff_Lymphocytes</t>
+  </si>
+  <si>
+    <t>CBCdiff_Monocytes</t>
+  </si>
+  <si>
+    <t>CBCdiff_Eosinophils</t>
+  </si>
+  <si>
+    <t>CBCdiff_Basophils</t>
+  </si>
+  <si>
+    <t>BMP_Na</t>
+  </si>
+  <si>
+    <t>BMP_K</t>
+  </si>
+  <si>
+    <t>BMP_Cl</t>
+  </si>
+  <si>
+    <t>BMP_CO2</t>
+  </si>
+  <si>
+    <t>BMP_BUN</t>
+  </si>
+  <si>
+    <t>BMP_Creatinine</t>
+  </si>
+  <si>
+    <t>BMP_Glucose</t>
+  </si>
+  <si>
+    <t>BMP_Calcium</t>
+  </si>
+  <si>
+    <t>CBCdiff</t>
+  </si>
+  <si>
+    <t>MCH</t>
+  </si>
+  <si>
+    <t>BMP</t>
+  </si>
+  <si>
+    <t>CMP_Na</t>
+  </si>
+  <si>
+    <t>CMP_K</t>
+  </si>
+  <si>
+    <t>CMP_Cl</t>
+  </si>
+  <si>
+    <t>CMP_CO2</t>
+  </si>
+  <si>
+    <t>CMP_BUN</t>
+  </si>
+  <si>
+    <t>CMP_Creatinine</t>
+  </si>
+  <si>
+    <t>CMP_Glucose</t>
+  </si>
+  <si>
+    <t>CMP_Calcium</t>
+  </si>
+  <si>
+    <t>CMP_AST</t>
+  </si>
+  <si>
+    <t>CMP_ALT</t>
+  </si>
+  <si>
+    <t>CMP_AlkPhos</t>
+  </si>
+  <si>
+    <t>CMP_TotBili</t>
+  </si>
+  <si>
+    <t>CMP_DirBili</t>
+  </si>
+  <si>
+    <t>PO4_PO4</t>
+  </si>
+  <si>
+    <t>Mg2_Mg2</t>
+  </si>
+  <si>
+    <t>LFTs_AST</t>
+  </si>
+  <si>
+    <t>LFTs_ALT</t>
+  </si>
+  <si>
+    <t>LFTs_AlkPhos</t>
+  </si>
+  <si>
+    <t>LFTs_TotBili</t>
+  </si>
+  <si>
+    <t>LFTs_DirBili</t>
+  </si>
+  <si>
+    <t>AmyLip_Amylase</t>
+  </si>
+  <si>
+    <t>AmyLip_Lipase</t>
+  </si>
+  <si>
+    <t>Troponin_TroponinI</t>
+  </si>
+  <si>
+    <t>BNP_BNP</t>
+  </si>
+  <si>
+    <t>D-dimer_D-dimer</t>
+  </si>
+  <si>
+    <t>Lactate_Lactate</t>
+  </si>
+  <si>
+    <t>CoagulationPanel_PTINR</t>
+  </si>
+  <si>
+    <t>CoagulationPanel_PTT</t>
+  </si>
+  <si>
+    <t>ABG_pH</t>
+  </si>
+  <si>
+    <t>ABG_paCO2</t>
+  </si>
+  <si>
+    <t>ABG_paO2</t>
+  </si>
+  <si>
+    <t>ABG_Bicarb</t>
+  </si>
+  <si>
+    <t>ABG_O2sat</t>
+  </si>
+  <si>
+    <t>VBG_pH</t>
+  </si>
+  <si>
+    <t>VBG_pvCO2</t>
+  </si>
+  <si>
+    <t>VBG_pvO2</t>
+  </si>
+  <si>
+    <t>VBG_Bicarb</t>
+  </si>
+  <si>
+    <t>VBG_O2sat</t>
+  </si>
+  <si>
+    <t>x 10^9/L</t>
+  </si>
+  <si>
+    <t>Mg2</t>
+  </si>
+  <si>
+    <t>PO4</t>
+  </si>
+  <si>
+    <t>AmyLip</t>
+  </si>
+  <si>
+    <t>D-dimer</t>
+  </si>
+  <si>
+    <t>CoagulationPanel</t>
+  </si>
+  <si>
+    <t>paCO2</t>
+  </si>
+  <si>
+    <t>paO2</t>
+  </si>
+  <si>
+    <t>O2sat</t>
+  </si>
+  <si>
+    <t>pvCO2</t>
+  </si>
+  <si>
+    <t>pvO2</t>
+  </si>
+  <si>
+    <t>Min_Norm</t>
+  </si>
+  <si>
+    <t>Max_Norm</t>
+  </si>
+  <si>
+    <t>male: 41, female: 36</t>
+  </si>
+  <si>
+    <t>male: 51, female: 47</t>
+  </si>
+  <si>
+    <t>male: 14, female: 12</t>
+  </si>
+  <si>
+    <t>male: 17, female: 16</t>
   </si>
 </sst>
 </file>
@@ -4115,6 +4360,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4571,6 +4817,311 @@
     <row r="60" spans="1:28" ht="12.75" x14ac:dyDescent="0.35">
       <c r="L60" s="1" t="s">
         <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A2:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" customWidth="1"/>
+    <col min="5" max="5" width="54.73046875" customWidth="1"/>
+    <col min="6" max="6" width="4.3984375" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="5.73046875" customWidth="1"/>
+    <col min="9" max="9" width="29.3984375" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" customWidth="1"/>
+    <col min="11" max="11" width="31.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="8" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>673</v>
+      </c>
+      <c r="G6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K19" s="8" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K20" s="8" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K21" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K22" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="K23" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -4585,9 +5136,10 @@
   </sheetPr>
   <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:BJ41"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5662,6 +6214,7 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8396,6 +8949,7 @@
     <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10482,6 +11036,7 @@
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AU19" sqref="AU19"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -10978,11 +11533,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54834C7C-FFC1-4FDA-AF9B-33C488204F5D}">
-  <dimension ref="A1:BJ22"/>
+  <dimension ref="A1:BJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AM6" sqref="AM6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -11971,7 +12527,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="17" spans="51:53" x14ac:dyDescent="0.35">
       <c r="AY17" s="6" t="s">
         <v>297</v>
       </c>
@@ -11980,40 +12536,6 @@
       </c>
       <c r="BA17" s="6" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1144</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>17000</v>
-      </c>
-      <c r="C22">
-        <v>45</v>
-      </c>
-      <c r="D22">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -12022,6 +12544,1645 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C648E6-513D-4FFF-82C3-7E94EB1BE2C3}">
+  <dimension ref="A1:BK66"/>
+  <sheetViews>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AY1" sqref="AY1"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="1">
+      <selection activeCell="F67" sqref="F67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="W1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="X1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>17000</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>17000</v>
+      </c>
+      <c r="G2">
+        <v>45</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>90</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>34</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>0.4</v>
+      </c>
+      <c r="P2">
+        <v>0.2</v>
+      </c>
+      <c r="Q2">
+        <v>40</v>
+      </c>
+      <c r="R2">
+        <v>140</v>
+      </c>
+      <c r="S2">
+        <v>4.2</v>
+      </c>
+      <c r="T2">
+        <v>100</v>
+      </c>
+      <c r="U2">
+        <v>27</v>
+      </c>
+      <c r="V2">
+        <v>14</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>84</v>
+      </c>
+      <c r="Y2">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Z2">
+        <v>140</v>
+      </c>
+      <c r="AA2">
+        <v>4.2</v>
+      </c>
+      <c r="AB2">
+        <v>100</v>
+      </c>
+      <c r="AC2">
+        <v>27</v>
+      </c>
+      <c r="AD2">
+        <v>14</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>84</v>
+      </c>
+      <c r="AG2">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
+      <c r="AN2">
+        <v>5</v>
+      </c>
+      <c r="AO2">
+        <v>34</v>
+      </c>
+      <c r="AP2">
+        <v>30</v>
+      </c>
+      <c r="AQ2">
+        <v>50</v>
+      </c>
+      <c r="AR2">
+        <v>0.5</v>
+      </c>
+      <c r="AS2">
+        <v>0.2</v>
+      </c>
+      <c r="AT2">
+        <v>60</v>
+      </c>
+      <c r="AU2">
+        <v>40</v>
+      </c>
+      <c r="AV2">
+        <v>0.01</v>
+      </c>
+      <c r="AW2">
+        <v>30</v>
+      </c>
+      <c r="AX2">
+        <v>0.02</v>
+      </c>
+      <c r="AY2">
+        <v>3</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>30</v>
+      </c>
+      <c r="BB2">
+        <v>7.46</v>
+      </c>
+      <c r="BC2">
+        <v>47</v>
+      </c>
+      <c r="BD2">
+        <v>98</v>
+      </c>
+      <c r="BE2">
+        <v>28</v>
+      </c>
+      <c r="BF2">
+        <v>99</v>
+      </c>
+      <c r="BG2">
+        <v>7.46</v>
+      </c>
+      <c r="BH2">
+        <v>50</v>
+      </c>
+      <c r="BI2">
+        <v>34</v>
+      </c>
+      <c r="BJ2">
+        <v>28</v>
+      </c>
+      <c r="BK2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5">
+        <v>3200</v>
+      </c>
+      <c r="F5">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8">
+        <v>150</v>
+      </c>
+      <c r="F8">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9">
+        <v>3200</v>
+      </c>
+      <c r="F9">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12">
+        <v>150</v>
+      </c>
+      <c r="F12">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E18">
+        <v>0.2</v>
+      </c>
+      <c r="F18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>135</v>
+      </c>
+      <c r="F21">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22">
+        <v>3.5</v>
+      </c>
+      <c r="F22">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>96</v>
+      </c>
+      <c r="F23">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27">
+        <v>79</v>
+      </c>
+      <c r="F27">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28">
+        <v>8.5</v>
+      </c>
+      <c r="F28">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29">
+        <v>135</v>
+      </c>
+      <c r="F29">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30">
+        <v>3.5</v>
+      </c>
+      <c r="F30">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31">
+        <v>96</v>
+      </c>
+      <c r="F31">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32">
+        <v>22</v>
+      </c>
+      <c r="F32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35">
+        <v>79</v>
+      </c>
+      <c r="F35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36">
+        <v>8.5</v>
+      </c>
+      <c r="F36">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39">
+        <v>30</v>
+      </c>
+      <c r="F39">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40">
+        <v>0.1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41">
+        <v>0.1</v>
+      </c>
+      <c r="F41">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42">
+        <v>1.7</v>
+      </c>
+      <c r="F42">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43">
+        <v>2.5</v>
+      </c>
+      <c r="F43">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46">
+        <v>30</v>
+      </c>
+      <c r="F46">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47">
+        <v>0.1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48">
+        <v>0.1</v>
+      </c>
+      <c r="F48">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54">
+        <v>0.4</v>
+      </c>
+      <c r="F54">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C55" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55">
+        <v>0.8</v>
+      </c>
+      <c r="F55">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C56" t="s">
+        <v>206</v>
+      </c>
+      <c r="D56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E56">
+        <v>25</v>
+      </c>
+      <c r="F56">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B57" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" t="s">
+        <v>211</v>
+      </c>
+      <c r="E57">
+        <v>7.37</v>
+      </c>
+      <c r="F57">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B58" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D58" t="s">
+        <v>221</v>
+      </c>
+      <c r="E58">
+        <v>35</v>
+      </c>
+      <c r="F58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B59" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D59" t="s">
+        <v>221</v>
+      </c>
+      <c r="E59">
+        <v>80</v>
+      </c>
+      <c r="F59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B60" t="s">
+        <v>195</v>
+      </c>
+      <c r="C60" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" t="s">
+        <v>238</v>
+      </c>
+      <c r="E60">
+        <v>23</v>
+      </c>
+      <c r="F60">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B61" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61">
+        <v>94</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B62" t="s">
+        <v>735</v>
+      </c>
+      <c r="C62" t="s">
+        <v>211</v>
+      </c>
+      <c r="E62">
+        <v>7.37</v>
+      </c>
+      <c r="F62">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B63" t="s">
+        <v>735</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D63" t="s">
+        <v>221</v>
+      </c>
+      <c r="E63">
+        <v>41</v>
+      </c>
+      <c r="F63">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B64" t="s">
+        <v>735</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D64" t="s">
+        <v>221</v>
+      </c>
+      <c r="E64">
+        <v>30</v>
+      </c>
+      <c r="F64">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B65" t="s">
+        <v>735</v>
+      </c>
+      <c r="C65" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" t="s">
+        <v>238</v>
+      </c>
+      <c r="E65">
+        <v>23</v>
+      </c>
+      <c r="F65">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B66" t="s">
+        <v>735</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D66" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66">
+        <v>94</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12031,6 +14192,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -12331,7 +14493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12341,6 +14503,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12420,308 +14583,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A2:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="5.59765625" customWidth="1"/>
-    <col min="5" max="5" width="54.73046875" customWidth="1"/>
-    <col min="6" max="6" width="4.3984375" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="5.73046875" customWidth="1"/>
-    <col min="9" max="9" width="29.3984375" customWidth="1"/>
-    <col min="10" max="10" width="5.73046875" customWidth="1"/>
-    <col min="11" max="11" width="31.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="1" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="8" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>673</v>
-      </c>
-      <c r="G6" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>675</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>680</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>683</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6" t="s">
-        <v>678</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>684</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F14" s="6" t="s">
-        <v>678</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>686</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H17" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>689</v>
-      </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H18" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K19" s="8" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K20" s="8" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K21" s="1" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K22" s="1" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="K23" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="D24" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>699</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>701</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
save components of lab to display
</commit_message>
<xml_diff>
--- a/data/PT Emergency Medicine v2.xlsx
+++ b/data/PT Emergency Medicine v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\court\OneDrive\Documents\GitHub\em-quiz-game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53ae2bac257da32/Documents/GitHub/em-quiz-game/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EAA2001E-80D0-41C0-A9D4-D0C07EAF3D4B}"/>
+  <xr:revisionPtr revIDLastSave="460" documentId="13_ncr:1_{7FD653CA-AA4F-4780-8232-870789B67D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7A87E82-79EE-466F-B18B-6D1ACF62B526}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="4" activeTab="6" xr2:uid="{E832494E-F55B-4BFD-B915-837CB7A7C282}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="7" xr2:uid="{E832494E-F55B-4BFD-B915-837CB7A7C282}"/>
   </bookViews>
   <sheets>
     <sheet name="Databases" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,17 @@
     <sheet name="Case Info" sheetId="4" r:id="rId5"/>
     <sheet name="Case1 labs" sheetId="9" r:id="rId6"/>
     <sheet name="Labs CSV format" sheetId="10" r:id="rId7"/>
-    <sheet name="CSV Case Info" sheetId="5" r:id="rId8"/>
-    <sheet name="GoalsTasks" sheetId="6" r:id="rId9"/>
-    <sheet name="Flow chart" sheetId="7" r:id="rId10"/>
+    <sheet name="Labs CSV Norms" sheetId="11" r:id="rId8"/>
+    <sheet name="CSV Case Info" sheetId="5" r:id="rId9"/>
+    <sheet name="GoalsTasks" sheetId="6" r:id="rId10"/>
+    <sheet name="Flow chart" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2678" uniqueCount="1254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="1258">
   <si>
     <t>values per American Board of Emergency Medicine</t>
   </si>
@@ -3947,6 +3948,18 @@
   </si>
   <si>
     <t>StrepScreen_Culture</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Quantitative</t>
+  </si>
+  <si>
+    <t>Qualitative</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -4899,6 +4912,95 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12603,9 +12705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C648E6-513D-4FFF-82C3-7E94EB1BE2C3}">
   <dimension ref="A1:CN95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -13162,1737 +13262,26 @@
         <v>748</v>
       </c>
     </row>
-    <row r="4" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1153</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5">
-        <v>3200</v>
-      </c>
-      <c r="F5">
-        <v>9800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1144</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1225</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1146</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8">
-        <v>150</v>
-      </c>
-      <c r="F8">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1147</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9">
-        <v>3200</v>
-      </c>
-      <c r="F9">
-        <v>9800</v>
-      </c>
-    </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1148</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1225</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12">
-        <v>150</v>
-      </c>
-      <c r="F12">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13">
-        <v>80</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1152</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14">
-        <v>28</v>
-      </c>
-      <c r="F14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1157</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C18" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E18">
-        <v>0.2</v>
-      </c>
-      <c r="F18">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E20">
-        <v>40</v>
-      </c>
-      <c r="F20">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21">
-        <v>135</v>
-      </c>
-      <c r="F21">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22">
-        <v>3.5</v>
-      </c>
-      <c r="F22">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23">
-        <v>96</v>
-      </c>
-      <c r="F23">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24">
-        <v>22</v>
-      </c>
-      <c r="F24">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25">
-        <v>6</v>
-      </c>
-      <c r="F25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C26" t="s">
-        <v>126</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26">
-        <v>0.5</v>
-      </c>
-      <c r="F26">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C27" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27">
-        <v>79</v>
-      </c>
-      <c r="F27">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28">
-        <v>8.5</v>
-      </c>
-      <c r="F28">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29">
-        <v>135</v>
-      </c>
-      <c r="F29">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>1174</v>
-      </c>
-      <c r="B30" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30">
-        <v>3.5</v>
-      </c>
-      <c r="F30">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>1175</v>
-      </c>
-      <c r="B31" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31">
-        <v>96</v>
-      </c>
-      <c r="F31">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B32" t="s">
-        <v>189</v>
-      </c>
-      <c r="C32" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32">
-        <v>22</v>
-      </c>
-      <c r="F32">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B33" t="s">
-        <v>189</v>
-      </c>
-      <c r="C33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33">
-        <v>6</v>
-      </c>
-      <c r="F33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>1178</v>
-      </c>
-      <c r="B34" t="s">
-        <v>189</v>
-      </c>
-      <c r="C34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34">
-        <v>0.5</v>
-      </c>
-      <c r="F34">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B35" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35">
-        <v>79</v>
-      </c>
-      <c r="F35">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>1180</v>
-      </c>
-      <c r="B36" t="s">
-        <v>189</v>
-      </c>
-      <c r="C36" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36">
-        <v>8.5</v>
-      </c>
-      <c r="F36">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>1181</v>
-      </c>
-      <c r="B37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C37" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37">
-        <v>6</v>
-      </c>
-      <c r="F37">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B38" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38">
-        <v>6</v>
-      </c>
-      <c r="F38">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>1183</v>
-      </c>
-      <c r="B39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39">
-        <v>30</v>
-      </c>
-      <c r="F39">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>1184</v>
-      </c>
-      <c r="B40" t="s">
-        <v>189</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40">
-        <v>0.1</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B41" t="s">
-        <v>189</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41">
-        <v>0.1</v>
-      </c>
-      <c r="F41">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42">
-        <v>1.7</v>
-      </c>
-      <c r="F42">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43">
-        <v>2.5</v>
-      </c>
-      <c r="F43">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44">
-        <v>6</v>
-      </c>
-      <c r="F44">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45">
-        <v>6</v>
-      </c>
-      <c r="F45">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46">
-        <v>30</v>
-      </c>
-      <c r="F46">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47">
-        <v>0.1</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48">
-        <v>0.1</v>
-      </c>
-      <c r="F48">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>1194</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C50" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>1196</v>
-      </c>
-      <c r="B52" t="s">
-        <v>168</v>
-      </c>
-      <c r="C52" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" t="s">
-        <v>171</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>1197</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D53" t="s">
-        <v>175</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>1198</v>
-      </c>
-      <c r="B54" t="s">
-        <v>176</v>
-      </c>
-      <c r="C54" t="s">
-        <v>176</v>
-      </c>
-      <c r="D54" t="s">
-        <v>72</v>
-      </c>
-      <c r="E54">
-        <v>0.4</v>
-      </c>
-      <c r="F54">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B55" t="s">
-        <v>730</v>
-      </c>
-      <c r="C55" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55">
-        <v>0.8</v>
-      </c>
-      <c r="F55">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>730</v>
-      </c>
-      <c r="C56" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" t="s">
-        <v>210</v>
-      </c>
-      <c r="E56">
-        <v>25</v>
-      </c>
-      <c r="F56">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B57" t="s">
-        <v>195</v>
-      </c>
-      <c r="C57" t="s">
-        <v>211</v>
-      </c>
-      <c r="E57">
-        <v>7.37</v>
-      </c>
-      <c r="F57">
-        <v>7.44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D58" t="s">
-        <v>221</v>
-      </c>
-      <c r="E58">
-        <v>35</v>
-      </c>
-      <c r="F58">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B59" t="s">
-        <v>195</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D59" t="s">
-        <v>221</v>
-      </c>
-      <c r="E59">
-        <v>80</v>
-      </c>
-      <c r="F59">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>1204</v>
-      </c>
-      <c r="B60" t="s">
-        <v>195</v>
-      </c>
-      <c r="C60" t="s">
-        <v>236</v>
-      </c>
-      <c r="D60" t="s">
-        <v>238</v>
-      </c>
-      <c r="E60">
-        <v>23</v>
-      </c>
-      <c r="F60">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B61" t="s">
-        <v>195</v>
-      </c>
-      <c r="C61" t="s">
-        <v>242</v>
-      </c>
-      <c r="D61" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61">
-        <v>94</v>
-      </c>
-      <c r="F61">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B62" t="s">
-        <v>735</v>
-      </c>
-      <c r="C62" t="s">
-        <v>211</v>
-      </c>
-      <c r="E62">
-        <v>7.37</v>
-      </c>
-      <c r="F62">
-        <v>7.44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>1207</v>
-      </c>
-      <c r="B63" t="s">
-        <v>735</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D63" t="s">
-        <v>221</v>
-      </c>
-      <c r="E63">
-        <v>41</v>
-      </c>
-      <c r="F63">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B64" t="s">
-        <v>735</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1220</v>
-      </c>
-      <c r="D64" t="s">
-        <v>221</v>
-      </c>
-      <c r="E64">
-        <v>30</v>
-      </c>
-      <c r="F64">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>1209</v>
-      </c>
-      <c r="B65" t="s">
-        <v>735</v>
-      </c>
-      <c r="C65" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" t="s">
-        <v>238</v>
-      </c>
-      <c r="E65">
-        <v>23</v>
-      </c>
-      <c r="F65">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B66" t="s">
-        <v>735</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D66" t="s">
-        <v>89</v>
-      </c>
-      <c r="E66">
-        <v>94</v>
-      </c>
-      <c r="F66">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B67" t="s">
-        <v>196</v>
-      </c>
-      <c r="C67" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" t="s">
-        <v>199</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B68" t="s">
-        <v>732</v>
-      </c>
-      <c r="C68" t="s">
-        <v>213</v>
-      </c>
-      <c r="E68" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B69" t="s">
-        <v>732</v>
-      </c>
-      <c r="C69" t="s">
-        <v>224</v>
-      </c>
-      <c r="E69" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F69" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B70" t="s">
-        <v>732</v>
-      </c>
-      <c r="C70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E70">
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="F70">
-        <v>1.032</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B71" t="s">
-        <v>732</v>
-      </c>
-      <c r="C71" t="s">
-        <v>211</v>
-      </c>
-      <c r="E71">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F71">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>1232</v>
-      </c>
-      <c r="B72" t="s">
-        <v>732</v>
-      </c>
-      <c r="C72" t="s">
-        <v>246</v>
-      </c>
-      <c r="E72" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F72" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B73" t="s">
-        <v>732</v>
-      </c>
-      <c r="C73" t="s">
-        <v>250</v>
-      </c>
-      <c r="D73" t="s">
-        <v>253</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B74" t="s">
-        <v>732</v>
-      </c>
-      <c r="C74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F74" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B75" t="s">
-        <v>732</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="E75" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F75" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B76" t="s">
-        <v>732</v>
-      </c>
-      <c r="C76" t="s">
-        <v>272</v>
-      </c>
-      <c r="E76" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F76" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B77" t="s">
-        <v>732</v>
-      </c>
-      <c r="C77" t="s">
-        <v>276</v>
-      </c>
-      <c r="E77" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F77" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B78" t="s">
-        <v>732</v>
-      </c>
-      <c r="C78" t="s">
-        <v>280</v>
-      </c>
-      <c r="E78" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F78" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>1239</v>
-      </c>
-      <c r="B79" t="s">
-        <v>732</v>
-      </c>
-      <c r="C79" t="s">
-        <v>289</v>
-      </c>
-      <c r="D79" t="s">
-        <v>294</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B80" t="s">
-        <v>732</v>
-      </c>
-      <c r="C80" t="s">
-        <v>297</v>
-      </c>
-      <c r="D80" t="s">
-        <v>294</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B81" t="s">
-        <v>731</v>
-      </c>
-      <c r="C81" t="s">
-        <v>731</v>
-      </c>
-      <c r="E81" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F81" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B82" t="s">
-        <v>731</v>
-      </c>
-      <c r="C82" t="s">
-        <v>215</v>
-      </c>
-      <c r="E82" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F82" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B83" t="s">
-        <v>731</v>
-      </c>
-      <c r="C83" t="s">
-        <v>228</v>
-      </c>
-      <c r="E83" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F83" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B84" t="s">
-        <v>731</v>
-      </c>
-      <c r="C84" t="s">
-        <v>233</v>
-      </c>
-      <c r="E84" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F84" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>1245</v>
-      </c>
-      <c r="B85" t="s">
-        <v>731</v>
-      </c>
-      <c r="C85" t="s">
-        <v>241</v>
-      </c>
-      <c r="E85" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F85" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B86" t="s">
-        <v>731</v>
-      </c>
-      <c r="C86" t="s">
-        <v>248</v>
-      </c>
-      <c r="E86" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F86" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B87" t="s">
-        <v>731</v>
-      </c>
-      <c r="C87" t="s">
-        <v>256</v>
-      </c>
-      <c r="E87" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F87" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B88" t="s">
-        <v>731</v>
-      </c>
-      <c r="C88" t="s">
-        <v>261</v>
-      </c>
-      <c r="E88" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F88" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B89" t="s">
-        <v>733</v>
-      </c>
-      <c r="E89" t="s">
-        <v>748</v>
-      </c>
-      <c r="F89" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B90" t="s">
-        <v>741</v>
-      </c>
-      <c r="E90" t="s">
-        <v>748</v>
-      </c>
-      <c r="F90" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B91" t="s">
-        <v>742</v>
-      </c>
-      <c r="E91" t="s">
-        <v>748</v>
-      </c>
-      <c r="F91" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>734</v>
-      </c>
-      <c r="B92" t="s">
-        <v>734</v>
-      </c>
-      <c r="E92" t="s">
-        <v>748</v>
-      </c>
-      <c r="F92" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>18</v>
-      </c>
-      <c r="B93" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" t="s">
-        <v>748</v>
-      </c>
-      <c r="F93" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B94" t="s">
-        <v>747</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="E94" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F94" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B95" t="s">
-        <v>747</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>746</v>
-      </c>
-      <c r="E95" t="s">
-        <v>748</v>
-      </c>
-      <c r="F95" t="s">
-        <v>748</v>
-      </c>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C94" s="16"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14900,6 +13289,2029 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993F0B8E-4974-4AD1-BDDB-EA42A692E363}">
+  <dimension ref="A1:G92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>3200</v>
+      </c>
+      <c r="F2">
+        <v>9800</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>150</v>
+      </c>
+      <c r="F5">
+        <v>450</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6">
+        <v>3200</v>
+      </c>
+      <c r="F6">
+        <v>9800</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>450</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E15">
+        <v>0.2</v>
+      </c>
+      <c r="F15">
+        <v>0.8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18">
+        <v>135</v>
+      </c>
+      <c r="F18">
+        <v>145</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19">
+        <v>3.5</v>
+      </c>
+      <c r="F19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20">
+        <v>96</v>
+      </c>
+      <c r="F20">
+        <v>106</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>22</v>
+      </c>
+      <c r="F21">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+      <c r="F23">
+        <v>1.2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24">
+        <v>79</v>
+      </c>
+      <c r="F24">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25">
+        <v>8.5</v>
+      </c>
+      <c r="F25">
+        <v>10.5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26">
+        <v>135</v>
+      </c>
+      <c r="F26">
+        <v>145</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27">
+        <v>3.5</v>
+      </c>
+      <c r="F27">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28">
+        <v>96</v>
+      </c>
+      <c r="F28">
+        <v>106</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29">
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <v>1.2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32">
+        <v>79</v>
+      </c>
+      <c r="F32">
+        <v>99</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33">
+        <v>8.5</v>
+      </c>
+      <c r="F33">
+        <v>10.5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36">
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <v>120</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37">
+        <v>0.1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38">
+        <v>0.1</v>
+      </c>
+      <c r="F38">
+        <v>0.4</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39">
+        <v>1.7</v>
+      </c>
+      <c r="F39">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40">
+        <v>2.5</v>
+      </c>
+      <c r="F40">
+        <v>4.8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43">
+        <v>30</v>
+      </c>
+      <c r="F43">
+        <v>120</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44">
+        <v>0.1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45">
+        <v>0.1</v>
+      </c>
+      <c r="F45">
+        <v>0.4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>130</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>95</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0.5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B49" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D50" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0.5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51">
+        <v>0.4</v>
+      </c>
+      <c r="F51">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B52" t="s">
+        <v>730</v>
+      </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52">
+        <v>0.8</v>
+      </c>
+      <c r="F52">
+        <v>1.2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B53" t="s">
+        <v>730</v>
+      </c>
+      <c r="C53" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" t="s">
+        <v>210</v>
+      </c>
+      <c r="E53">
+        <v>25</v>
+      </c>
+      <c r="F53">
+        <v>35</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B54" t="s">
+        <v>195</v>
+      </c>
+      <c r="C54" t="s">
+        <v>211</v>
+      </c>
+      <c r="E54">
+        <v>7.37</v>
+      </c>
+      <c r="F54">
+        <v>7.44</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B55" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D55" t="s">
+        <v>221</v>
+      </c>
+      <c r="E55">
+        <v>35</v>
+      </c>
+      <c r="F55">
+        <v>45</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B56" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D56" t="s">
+        <v>221</v>
+      </c>
+      <c r="E56">
+        <v>80</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+      <c r="G56" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B57" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" t="s">
+        <v>236</v>
+      </c>
+      <c r="D57" t="s">
+        <v>238</v>
+      </c>
+      <c r="E57">
+        <v>23</v>
+      </c>
+      <c r="F57">
+        <v>28</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B58" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58">
+        <v>94</v>
+      </c>
+      <c r="F58">
+        <v>100</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B59" t="s">
+        <v>735</v>
+      </c>
+      <c r="C59" t="s">
+        <v>211</v>
+      </c>
+      <c r="E59">
+        <v>7.37</v>
+      </c>
+      <c r="F59">
+        <v>7.44</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B60" t="s">
+        <v>735</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D60" t="s">
+        <v>221</v>
+      </c>
+      <c r="E60">
+        <v>41</v>
+      </c>
+      <c r="F60">
+        <v>51</v>
+      </c>
+      <c r="G60" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B61" t="s">
+        <v>735</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D61" t="s">
+        <v>221</v>
+      </c>
+      <c r="E61">
+        <v>30</v>
+      </c>
+      <c r="F61">
+        <v>40</v>
+      </c>
+      <c r="G61" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B62" t="s">
+        <v>735</v>
+      </c>
+      <c r="C62" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" t="s">
+        <v>238</v>
+      </c>
+      <c r="E62">
+        <v>23</v>
+      </c>
+      <c r="F62">
+        <v>28</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B63" t="s">
+        <v>735</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D63" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63">
+        <v>94</v>
+      </c>
+      <c r="F63">
+        <v>100</v>
+      </c>
+      <c r="G63" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B65" t="s">
+        <v>732</v>
+      </c>
+      <c r="C65" t="s">
+        <v>213</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G65" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B66" t="s">
+        <v>732</v>
+      </c>
+      <c r="C66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B67" t="s">
+        <v>732</v>
+      </c>
+      <c r="C67" t="s">
+        <v>230</v>
+      </c>
+      <c r="E67">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="F67">
+        <v>1.032</v>
+      </c>
+      <c r="G67" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B68" t="s">
+        <v>732</v>
+      </c>
+      <c r="C68" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F68">
+        <v>8</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B69" t="s">
+        <v>732</v>
+      </c>
+      <c r="C69" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B70" t="s">
+        <v>732</v>
+      </c>
+      <c r="C70" t="s">
+        <v>250</v>
+      </c>
+      <c r="D70" t="s">
+        <v>253</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>150</v>
+      </c>
+      <c r="G70" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B71" t="s">
+        <v>732</v>
+      </c>
+      <c r="C71" t="s">
+        <v>132</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G71" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B72" t="s">
+        <v>732</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G72" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B73" t="s">
+        <v>732</v>
+      </c>
+      <c r="C73" t="s">
+        <v>272</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G73" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B74" t="s">
+        <v>732</v>
+      </c>
+      <c r="C74" t="s">
+        <v>276</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G74" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B75" t="s">
+        <v>732</v>
+      </c>
+      <c r="C75" t="s">
+        <v>280</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G75" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B76" t="s">
+        <v>732</v>
+      </c>
+      <c r="C76" t="s">
+        <v>289</v>
+      </c>
+      <c r="D76" t="s">
+        <v>294</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B77" t="s">
+        <v>732</v>
+      </c>
+      <c r="C77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D77" t="s">
+        <v>294</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>4</v>
+      </c>
+      <c r="G77" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B78" t="s">
+        <v>731</v>
+      </c>
+      <c r="C78" t="s">
+        <v>731</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G78" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B79" t="s">
+        <v>731</v>
+      </c>
+      <c r="C79" t="s">
+        <v>215</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G79" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B80" t="s">
+        <v>731</v>
+      </c>
+      <c r="C80" t="s">
+        <v>228</v>
+      </c>
+      <c r="E80" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G80" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B81" t="s">
+        <v>731</v>
+      </c>
+      <c r="C81" t="s">
+        <v>233</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G81" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B82" t="s">
+        <v>731</v>
+      </c>
+      <c r="C82" t="s">
+        <v>241</v>
+      </c>
+      <c r="E82" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G82" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B83" t="s">
+        <v>731</v>
+      </c>
+      <c r="C83" t="s">
+        <v>248</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G83" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B84" t="s">
+        <v>731</v>
+      </c>
+      <c r="C84" t="s">
+        <v>256</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G84" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B85" t="s">
+        <v>731</v>
+      </c>
+      <c r="C85" t="s">
+        <v>261</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G85" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B86" t="s">
+        <v>733</v>
+      </c>
+      <c r="E86" t="s">
+        <v>748</v>
+      </c>
+      <c r="F86" t="s">
+        <v>748</v>
+      </c>
+      <c r="G86" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B87" t="s">
+        <v>741</v>
+      </c>
+      <c r="E87" t="s">
+        <v>748</v>
+      </c>
+      <c r="F87" t="s">
+        <v>748</v>
+      </c>
+      <c r="G87" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B88" t="s">
+        <v>742</v>
+      </c>
+      <c r="E88" t="s">
+        <v>748</v>
+      </c>
+      <c r="F88" t="s">
+        <v>748</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>734</v>
+      </c>
+      <c r="B89" t="s">
+        <v>734</v>
+      </c>
+      <c r="E89" t="s">
+        <v>748</v>
+      </c>
+      <c r="F89" t="s">
+        <v>748</v>
+      </c>
+      <c r="G89" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" t="s">
+        <v>748</v>
+      </c>
+      <c r="F90" t="s">
+        <v>748</v>
+      </c>
+      <c r="G90" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B91" t="s">
+        <v>747</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>745</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G91" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B92" t="s">
+        <v>747</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>746</v>
+      </c>
+      <c r="E92" t="s">
+        <v>748</v>
+      </c>
+      <c r="F92" t="s">
+        <v>748</v>
+      </c>
+      <c r="G92" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -15205,93 +15617,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32.59765625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>655</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>